<commit_message>
Add check list for Home page, Shopping cart and Checkout page
</commit_message>
<xml_diff>
--- a/Checklists/Checklist for E-commerce.xlsx
+++ b/Checklists/Checklist for E-commerce.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373EF95A-7DEB-4144-97FE-7CB8D136B186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5584FFB8-FE7C-4456-8DAC-4C79AD5E85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,29 +25,163 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Test Name</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Check list for https://dominos.ua/uk/kyiv/(as a example)</t>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>All controls are being displayed properly</t>
+  </si>
+  <si>
+    <t>Click to login, new user registration and other buttons (or links) are working as expected</t>
+  </si>
+  <si>
+    <t>Product filtering functionality is working as expected</t>
+  </si>
+  <si>
+    <t>Products are displayed on home page</t>
+  </si>
+  <si>
+    <t>Home page is displayed after login</t>
+  </si>
+  <si>
+    <t>User profile section is present on home page</t>
+  </si>
+  <si>
+    <t>Clicking the logo leads to home page</t>
+  </si>
+  <si>
+    <t>Appearance and functionality on different browsers</t>
+  </si>
+  <si>
+    <t>Carousell of highlight offer works as expected</t>
+  </si>
+  <si>
+    <t>Product details are displayed(name, content, price etc.)</t>
+  </si>
+  <si>
+    <t>All the variants of products are displayed("Стандартна", "Велика" etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shopping cart </t>
+  </si>
+  <si>
+    <t>Adding item to cart</t>
+  </si>
+  <si>
+    <t>Adding several items to cart</t>
+  </si>
+  <si>
+    <t>Changing  item quantity</t>
+  </si>
+  <si>
+    <t>Removing item from cart</t>
+  </si>
+  <si>
+    <t>Link for appropriate test case</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>No run</t>
+  </si>
+  <si>
+    <t>User is able to continue shopping after adding items to cart</t>
+  </si>
+  <si>
+    <t>User is not able to add items in cart beyond a certain limit</t>
+  </si>
+  <si>
+    <t>Items in cart are present if user logs out and logs in again</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Checkout page</t>
+  </si>
+  <si>
+    <t>User is able to choose the desired payment option</t>
+  </si>
+  <si>
+    <t>The reviews of the relevant products are displayed properly on the page</t>
+  </si>
+  <si>
+    <t>Delivery cost displayed if one item present</t>
+  </si>
+  <si>
+    <t>User directed to home page after checkout</t>
+  </si>
+  <si>
+    <t>"Телефон", "E-mail", "Вулиця" "Тип оплати" are mandatory fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different payment options are displayed </t>
+  </si>
+  <si>
+    <t>Alignment on home page is as expected</t>
+  </si>
+  <si>
+    <t>Products displayed on home page are categorized</t>
+  </si>
+  <si>
+    <t>Contact info is located on footer</t>
+  </si>
+  <si>
+    <t>On successful order user receives E-mail and text message with unique order number</t>
+  </si>
+  <si>
+    <t>Checklist for https://dominos.ua/uk/kyiv/(as a example)</t>
+  </si>
+  <si>
+    <t>Checking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,8 +195,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,7 +222,40 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -100,17 +284,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,22 +608,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
+      <c r="A1" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -412,137 +631,388 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="11">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="12">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="12">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="12">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="12">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>25</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>27</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>28</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D19" r:id="rId1" xr:uid="{BAD4745B-428A-4131-ABB4-45495269F0BE}"/>
+    <hyperlink ref="D20:D22" r:id="rId2" display="Link for appropriate test case" xr:uid="{A54DDE45-AE53-44F9-8B57-2206DEA42E0D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update status for checkings
</commit_message>
<xml_diff>
--- a/Checklists/Checklist for E-commerce.xlsx
+++ b/Checklists/Checklist for E-commerce.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5584FFB8-FE7C-4456-8DAC-4C79AD5E85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248C98A-7B9B-491D-BC8F-28065E6B4262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>No run</t>
-  </si>
-  <si>
     <t>User is able to continue shopping after adding items to cart</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Checking</t>
+  </si>
+  <si>
+    <t>Not run</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -656,7 +656,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -668,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -692,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4"/>
     </row>
@@ -701,10 +701,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4"/>
     </row>
@@ -713,10 +713,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4"/>
     </row>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -740,7 +740,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -752,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -764,7 +764,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4"/>
     </row>
@@ -773,10 +773,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4"/>
     </row>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -800,7 +800,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -812,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -885,10 +885,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -897,10 +897,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -909,17 +909,17 @@
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -928,10 +928,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -940,10 +940,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -952,10 +952,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D29" s="2"/>
     </row>
@@ -964,10 +964,10 @@
         <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -976,10 +976,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D31" s="2"/>
     </row>
@@ -988,10 +988,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -1000,10 +1000,10 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2"/>
     </row>

</xml_diff>

<commit_message>
Change status for checklist(e-commerce)
</commit_message>
<xml_diff>
--- a/Checklists/Checklist for E-commerce.xlsx
+++ b/Checklists/Checklist for E-commerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248C98A-7B9B-491D-BC8F-28065E6B4262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AA2DD9-7775-424B-876F-C88E6699EC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
     <t>Checking</t>
   </si>
   <si>
-    <t>Not run</t>
+    <t>Not tested</t>
   </si>
 </sst>
 </file>
@@ -611,13 +611,14 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="82" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>